<commit_message>
Bổ sung bug report
</commit_message>
<xml_diff>
--- a/Documents/Bug Report.xlsx
+++ b/Documents/Bug Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuti\Desktop\113\vuong + vu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuti\Documents\GitHub\EVTranslator\EVTranslator\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Function name</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -61,58 +55,70 @@
     <t>Nên kiểm tra DB từ forever</t>
   </si>
   <si>
-    <t>Lỗi khá nghiêm trọng</t>
-  </si>
-  <si>
-    <t>Lỗi dừng chương trình</t>
-  </si>
-  <si>
-    <t>Lỗi dịch ra kết quả Anh Việt Lẫn Lộn</t>
-  </si>
-  <si>
     <t>Đầu vào : it is ranining</t>
   </si>
   <si>
-    <t>Đầu ra : cái đó là raining</t>
-  </si>
-  <si>
-    <t>Lỗi về sữ liệu, hoặc thuật toán có nhầm lẫn.</t>
-  </si>
-  <si>
-    <t>Lỗi dịch ra kết quả không đúng</t>
-  </si>
-  <si>
     <t>Đầu vào : good bye</t>
   </si>
   <si>
     <t>Đầu ra : hay cái phụ</t>
   </si>
   <si>
-    <t>Lỗi về DB</t>
-  </si>
-  <si>
-    <t>Lỗi chon tin nhắn để dịch là tin tổng tiếng việt dài quá bị dừng chương trình</t>
-  </si>
-  <si>
     <t>Đầu vào là tin nhắn tiếng việt của tổng đài, chương trình bị dừng</t>
   </si>
   <si>
     <t>chương trình bị văng bug, dừng</t>
   </si>
   <si>
-    <t>Lỗi về sử lý tin nhắn quá dài</t>
-  </si>
-  <si>
-    <t>Lỗi tạo thư mục trùng tên vân tạo được</t>
-  </si>
-  <si>
     <t>Thư mục đã tồn tại, tạo thư mục giống tên vân tạo được</t>
   </si>
   <si>
     <t>Tạo được thư lục giống tên</t>
   </si>
   <si>
-    <t>Chưa kiểm tra điều kiện trùng tên thư mục yêu thích</t>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>Developer fix bug</t>
+  </si>
+  <si>
+    <t>Trần Trọng Thanh Tùng</t>
+  </si>
+  <si>
+    <t>TC_FT_01</t>
+  </si>
+  <si>
+    <t>TC_FT_06</t>
+  </si>
+  <si>
+    <t>TC_FT_14</t>
+  </si>
+  <si>
+    <t>Dịch 1 câu hỏi tiếng anh thành công</t>
+  </si>
+  <si>
+    <t>Dịch 1 tin nhắn SMS thành công</t>
+  </si>
+  <si>
+    <t>Tạo thư mục chủ đề thành công</t>
+  </si>
+  <si>
+    <t>DỊch ra tiếng việt anh lẫn lộn: "It is raining"</t>
+  </si>
+  <si>
+    <t>Dịch 2 đoạn văn thì chương trình tự động thoát</t>
+  </si>
+  <si>
+    <t>TMVuong</t>
+  </si>
+  <si>
+    <t>TC_FT_08</t>
+  </si>
+  <si>
+    <t>Lưu lịch sử câu đã dịch thành công.</t>
+  </si>
+  <si>
+    <t>Lưu câu đã lưu nhưng vẫn cho phép lưu</t>
   </si>
 </sst>
 </file>
@@ -163,26 +169,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
@@ -219,33 +252,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="9"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -269,8 +275,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -285,15 +291,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:G6" totalsRowShown="0">
-  <tableColumns count="7">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Function name" dataDxfId="3"/>
-    <tableColumn id="3" name="Problem summary" dataDxfId="2"/>
-    <tableColumn id="4" name="How to reproduce it" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H8" totalsRowShown="0">
+  <tableColumns count="8">
+    <tableColumn id="1" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" name="Function name" dataDxfId="0"/>
+    <tableColumn id="3" name="Problem summary" dataDxfId="4"/>
+    <tableColumn id="4" name="How to reproduce it" dataDxfId="3"/>
     <tableColumn id="5" name="Reported by"/>
-    <tableColumn id="6" name="Date" dataDxfId="0"/>
+    <tableColumn id="6" name="Date" dataDxfId="2"/>
     <tableColumn id="8" name="Status"/>
+    <tableColumn id="7" name="Developer fix bug"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,165 +593,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="68.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>42347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3">
+        <v>42347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3">
+        <v>42347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5">
-        <v>42259</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3">
+        <v>42347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5">
-        <v>42259</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3">
+        <v>42347</v>
+      </c>
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="H6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5">
-        <v>42259</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5">
-        <v>42259</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5">
-        <v>42259</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F7" s="3">
+        <v>42348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3">
+        <v>42348</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>